<commit_message>
Forced update with latest changes
</commit_message>
<xml_diff>
--- a/uploads/underground_list.xlsx
+++ b/uploads/underground_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alian\Desktop\ZamoraInventoryAnalyzer\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F0F0A0-AEF9-4B35-BF39-E389A8FE9970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80863FE5-B32E-4AEA-B58D-D73E52BEB277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1509" yWindow="1509" windowWidth="19268" windowHeight="16860" xr2:uid="{E8F0A0FA-43CC-4D96-937C-CEB14916B8E6}"/>
+    <workbookView xWindow="1509" yWindow="934" windowWidth="19268" windowHeight="16860" xr2:uid="{E8F0A0FA-43CC-4D96-937C-CEB14916B8E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">CLOSET BEND PVCDWV 4 x 3 </t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t xml:space="preserve">GALLON PURPLE PRIMER </t>
+  </si>
+  <si>
+    <t>Product Description</t>
   </si>
 </sst>
 </file>
@@ -208,6 +211,16 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AB1ED49-4472-450F-81AE-B5C82944D501}" name="Table1" displayName="Table1" ref="A1:A42" totalsRowShown="0">
+  <autoFilter ref="A1:A42" xr:uid="{1AB1ED49-4472-450F-81AE-B5C82944D501}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{658687D8-A4CD-4EDF-A0E1-FD02E44D42CA}" name="Product Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E2D337-EE11-4539-811D-4A8F2DC69A25}">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -540,211 +553,219 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>